<commit_message>
presented version tweaks to the templat
</commit_message>
<xml_diff>
--- a/Template.xlsx
+++ b/Template.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Statystyki marketingu w social media</t>
   </si>
@@ -52,6 +52,9 @@
   <si>
     <t>Średnia liczba lajków:</t>
   </si>
+  <si>
+    <t>Analiza:</t>
+  </si>
 </sst>
 </file>
 
@@ -60,7 +63,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-415]d\ mmm;@"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -145,6 +148,23 @@
       <charset val="238"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color theme="2" tint="-0.89999084444715716"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="2" tint="-0.89999084444715716"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -172,7 +192,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -201,36 +221,45 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="hair">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="medium">
+      <left style="hair">
+        <color indexed="64"/>
+      </left>
+      <right style="hair">
         <color indexed="64"/>
       </right>
-      <top style="medium">
+      <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
+      <left style="hair">
         <color indexed="64"/>
       </left>
       <right style="hair">
         <color indexed="64"/>
       </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color indexed="64"/>
+      </left>
+      <right/>
       <top/>
       <bottom/>
       <diagonal/>
@@ -238,9 +267,58 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
       <top style="medium">
         <color indexed="64"/>
       </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -251,56 +329,8 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
+      <top/>
       <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="hair">
-        <color indexed="64"/>
-      </left>
-      <right style="hair">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="hair">
-        <color indexed="64"/>
-      </left>
-      <right style="hair">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="hair">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -310,10 +340,8 @@
         <color indexed="64"/>
       </left>
       <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
+      <top/>
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -322,18 +350,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -342,23 +365,22 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -368,41 +390,128 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="8">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -761,17 +870,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L42"/>
+  <dimension ref="A1:L57"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.140625" customWidth="1"/>
-    <col min="2" max="2" width="6.42578125" style="21" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="2" max="2" width="6.42578125" style="16" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" customWidth="1"/>
     <col min="4" max="4" width="46" customWidth="1"/>
     <col min="5" max="5" width="9.42578125" customWidth="1"/>
     <col min="6" max="6" width="14.7109375" customWidth="1"/>
@@ -780,7 +889,7 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
-      <c r="B1" s="16"/>
+      <c r="B1" s="12"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -794,7 +903,7 @@
     </row>
     <row r="2" spans="1:12" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="13" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="1"/>
@@ -809,8 +918,8 @@
       <c r="L2" s="1"/>
     </row>
     <row r="3" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="12"/>
-      <c r="B3" s="18"/>
+      <c r="A3" s="9"/>
+      <c r="B3" s="14"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -823,431 +932,775 @@
       <c r="L3" s="1"/>
     </row>
     <row r="4" spans="1:12" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="12"/>
-      <c r="B4" s="19"/>
-      <c r="C4" s="4" t="s">
+      <c r="A4" s="9"/>
+      <c r="B4" s="26"/>
+      <c r="C4" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="22"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="3"/>
-    </row>
-    <row r="5" spans="1:12" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="12"/>
-      <c r="B5" s="23"/>
-      <c r="C5" s="4"/>
-      <c r="E5" s="24" t="s">
+      <c r="D4" s="27"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="20"/>
+      <c r="K4" s="20"/>
+      <c r="L4" s="21"/>
+    </row>
+    <row r="5" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="9"/>
+      <c r="B5" s="17"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="2"/>
-      <c r="G5" s="24" t="str">
-        <f>IF(NOT(ISERROR(AVERAGE(E7:E100))),AVERAGE(E7:E100)," ")</f>
+      <c r="F5" s="20"/>
+      <c r="G5" s="19" t="str">
+        <f>IF(NOT(ISERROR(AVERAGE(E8:E101))),AVERAGE(E8:E101)," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H5" s="24"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
-      <c r="L5" s="3"/>
-    </row>
-    <row r="6" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-      <c r="B6" s="28" t="s">
+      <c r="H5" s="19"/>
+      <c r="I5" s="20"/>
+      <c r="J5" s="20"/>
+      <c r="K5" s="20"/>
+      <c r="L5" s="21"/>
+    </row>
+    <row r="6" spans="1:12" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="9"/>
+      <c r="B6" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="31"/>
+      <c r="D6" s="28" t="str">
+        <f>IF(COUNTIF(D8:D51,"*video*"),"Posty zawierające filmy wydają się trafiać do większej liczby osób.",IF(SUM(E8:G10)&lt;(0.7*SUM(E11:G13)),"Wygląda na to, że ostatnie posty docierają do mniejszej liczby osób niż wcześniejsze.",IF(SUM(E8:G10)&gt;(1.2*SUM(E11:G13)),"Wygląda na to, że ostatnie posty docierają do wiekszej liczby osób niż wcześniejsze."," ")))</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="E6" s="28"/>
+      <c r="F6" s="28"/>
+      <c r="G6" s="28"/>
+      <c r="H6" s="28"/>
+      <c r="I6" s="28"/>
+      <c r="J6" s="28"/>
+      <c r="K6" s="28"/>
+      <c r="L6" s="29"/>
+    </row>
+    <row r="7" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="25" t="s">
+      <c r="C7" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="25" t="s">
+      <c r="D7" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="25" t="s">
+      <c r="E7" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="25" t="s">
+      <c r="F7" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="G6" s="25" t="s">
+      <c r="G7" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="H6" s="26"/>
-      <c r="I6" s="26"/>
-      <c r="J6" s="26"/>
-      <c r="K6" s="26"/>
-      <c r="L6" s="27"/>
-    </row>
-    <row r="7" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-      <c r="B7" s="20"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
-      <c r="J7" s="7"/>
-      <c r="K7" s="7"/>
-      <c r="L7" s="8"/>
+      <c r="H7" s="24"/>
+      <c r="I7" s="24"/>
+      <c r="J7" s="24"/>
+      <c r="K7" s="24"/>
+      <c r="L7" s="25"/>
     </row>
     <row r="8" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
-      <c r="B8" s="20"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7"/>
-      <c r="K8" s="7"/>
-      <c r="L8" s="8"/>
+      <c r="B8" s="15"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="5"/>
     </row>
     <row r="9" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
-      <c r="B9" s="20"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="7"/>
-      <c r="J9" s="7"/>
-      <c r="K9" s="7"/>
-      <c r="L9" s="8"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="4"/>
+      <c r="K9" s="4"/>
+      <c r="L9" s="5"/>
     </row>
     <row r="10" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
-      <c r="B10" s="20"/>
-      <c r="C10" s="14"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="7"/>
-      <c r="J10" s="7"/>
-      <c r="K10" s="7"/>
-      <c r="L10" s="8"/>
+      <c r="B10" s="15"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4"/>
+      <c r="K10" s="4"/>
+      <c r="L10" s="5"/>
     </row>
     <row r="11" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
-      <c r="B11" s="20"/>
-      <c r="C11" s="14"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="10"/>
-      <c r="H11" s="7"/>
-      <c r="I11" s="7"/>
-      <c r="J11" s="7"/>
-      <c r="K11" s="7"/>
-      <c r="L11" s="8"/>
+      <c r="B11" s="15"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="4"/>
+      <c r="K11" s="4"/>
+      <c r="L11" s="5"/>
     </row>
     <row r="12" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
-      <c r="B12" s="20"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="7"/>
-      <c r="I12" s="7"/>
-      <c r="J12" s="7"/>
-      <c r="K12" s="7"/>
-      <c r="L12" s="8"/>
+      <c r="B12" s="15"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4"/>
+      <c r="L12" s="5"/>
     </row>
     <row r="13" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
-      <c r="B13" s="20"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10"/>
-      <c r="H13" s="7"/>
-      <c r="I13" s="7"/>
-      <c r="J13" s="7"/>
-      <c r="K13" s="7"/>
-      <c r="L13" s="8"/>
+      <c r="B13" s="15"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="4"/>
+      <c r="K13" s="4"/>
+      <c r="L13" s="5"/>
     </row>
     <row r="14" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
-      <c r="B14" s="20"/>
-      <c r="C14" s="14"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="7"/>
-      <c r="I14" s="7"/>
-      <c r="J14" s="7"/>
-      <c r="K14" s="7"/>
-      <c r="L14" s="8"/>
+      <c r="B14" s="15"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
+      <c r="J14" s="4"/>
+      <c r="K14" s="4"/>
+      <c r="L14" s="5"/>
     </row>
     <row r="15" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
-      <c r="B15" s="20"/>
-      <c r="C15" s="14"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="10"/>
-      <c r="G15" s="10"/>
-      <c r="H15" s="7"/>
-      <c r="I15" s="7"/>
-      <c r="J15" s="7"/>
-      <c r="K15" s="7"/>
-      <c r="L15" s="8"/>
+      <c r="B15" s="15"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4"/>
+      <c r="J15" s="4"/>
+      <c r="K15" s="4"/>
+      <c r="L15" s="5"/>
     </row>
     <row r="16" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
-      <c r="B16" s="20"/>
-      <c r="C16" s="14"/>
-      <c r="D16" s="9"/>
-      <c r="E16" s="10"/>
-      <c r="F16" s="10"/>
-      <c r="G16" s="10"/>
-      <c r="H16" s="7"/>
-      <c r="I16" s="7"/>
-      <c r="J16" s="7"/>
-      <c r="K16" s="7"/>
-      <c r="L16" s="8"/>
+      <c r="B16" s="15"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4"/>
+      <c r="J16" s="4"/>
+      <c r="K16" s="4"/>
+      <c r="L16" s="5"/>
     </row>
     <row r="17" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
-      <c r="B17" s="20"/>
-      <c r="C17" s="14"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="10"/>
-      <c r="F17" s="10"/>
-      <c r="G17" s="10"/>
-      <c r="H17" s="11"/>
-      <c r="I17" s="7"/>
-      <c r="J17" s="7"/>
-      <c r="K17" s="7"/>
-      <c r="L17" s="8"/>
+      <c r="B17" s="15"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="4"/>
+      <c r="K17" s="4"/>
+      <c r="L17" s="5"/>
     </row>
     <row r="18" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
-      <c r="B18" s="20"/>
-      <c r="C18" s="14"/>
-      <c r="D18" s="9"/>
-      <c r="E18" s="10"/>
-      <c r="F18" s="10"/>
-      <c r="G18" s="10"/>
-      <c r="H18" s="7"/>
-      <c r="I18" s="7"/>
-      <c r="J18" s="7"/>
-      <c r="K18" s="7"/>
-      <c r="L18" s="8"/>
+      <c r="B18" s="15"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="8"/>
+      <c r="I18" s="4"/>
+      <c r="J18" s="4"/>
+      <c r="K18" s="4"/>
+      <c r="L18" s="5"/>
     </row>
     <row r="19" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
-      <c r="B19" s="20"/>
-      <c r="C19" s="14"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="10"/>
-      <c r="F19" s="10"/>
-      <c r="G19" s="10"/>
-      <c r="H19" s="7"/>
-      <c r="I19" s="7"/>
-      <c r="J19" s="7"/>
-      <c r="K19" s="7"/>
-      <c r="L19" s="8"/>
+      <c r="B19" s="15"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="4"/>
+      <c r="J19" s="4"/>
+      <c r="K19" s="4"/>
+      <c r="L19" s="5"/>
     </row>
     <row r="20" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
-      <c r="B20" s="20"/>
-      <c r="C20" s="14"/>
-      <c r="D20" s="9"/>
-      <c r="E20" s="10"/>
-      <c r="F20" s="10"/>
-      <c r="G20" s="10"/>
-      <c r="H20" s="11"/>
-      <c r="I20" s="7"/>
-      <c r="J20" s="7"/>
-      <c r="K20" s="7"/>
-      <c r="L20" s="8"/>
+      <c r="B20" s="15"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="4"/>
+      <c r="J20" s="4"/>
+      <c r="K20" s="4"/>
+      <c r="L20" s="5"/>
     </row>
     <row r="21" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
-      <c r="B21" s="20"/>
-      <c r="C21" s="14"/>
-      <c r="D21" s="9"/>
-      <c r="E21" s="10"/>
-      <c r="F21" s="10"/>
-      <c r="G21" s="10"/>
-      <c r="H21" s="7"/>
-      <c r="I21" s="7"/>
-      <c r="J21" s="7"/>
-      <c r="K21" s="7"/>
-      <c r="L21" s="8"/>
+      <c r="B21" s="15"/>
+      <c r="C21" s="11"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="8"/>
+      <c r="I21" s="4"/>
+      <c r="J21" s="4"/>
+      <c r="K21" s="4"/>
+      <c r="L21" s="5"/>
     </row>
     <row r="22" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
-      <c r="B22" s="20"/>
-      <c r="C22" s="14"/>
-      <c r="D22" s="9"/>
-      <c r="E22" s="10"/>
-      <c r="F22" s="10"/>
-      <c r="G22" s="10"/>
-      <c r="H22" s="7"/>
-      <c r="I22" s="7"/>
-      <c r="J22" s="7"/>
-      <c r="K22" s="7"/>
-      <c r="L22" s="8"/>
+      <c r="B22" s="15"/>
+      <c r="C22" s="11"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="7"/>
+      <c r="H22" s="4"/>
+      <c r="I22" s="4"/>
+      <c r="J22" s="4"/>
+      <c r="K22" s="4"/>
+      <c r="L22" s="5"/>
     </row>
     <row r="23" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
-      <c r="B23" s="20"/>
-      <c r="C23" s="14"/>
-      <c r="D23" s="9"/>
-      <c r="E23" s="10"/>
-      <c r="F23" s="10"/>
-      <c r="G23" s="10"/>
-      <c r="H23" s="11"/>
-      <c r="I23" s="7"/>
-      <c r="J23" s="7"/>
-      <c r="K23" s="7"/>
-      <c r="L23" s="8"/>
+      <c r="B23" s="15"/>
+      <c r="C23" s="11"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="7"/>
+      <c r="G23" s="7"/>
+      <c r="H23" s="4"/>
+      <c r="I23" s="4"/>
+      <c r="J23" s="4"/>
+      <c r="K23" s="4"/>
+      <c r="L23" s="5"/>
     </row>
     <row r="24" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="20"/>
-      <c r="C24" s="14"/>
-      <c r="D24" s="9"/>
-      <c r="E24" s="10"/>
-      <c r="F24" s="10"/>
-      <c r="G24" s="10"/>
-      <c r="H24" s="7"/>
-      <c r="I24" s="7"/>
-      <c r="J24" s="7"/>
-      <c r="K24" s="7"/>
-      <c r="L24" s="8"/>
+      <c r="A24" s="1"/>
+      <c r="B24" s="15"/>
+      <c r="C24" s="11"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="7"/>
+      <c r="H24" s="8"/>
+      <c r="I24" s="4"/>
+      <c r="J24" s="4"/>
+      <c r="K24" s="4"/>
+      <c r="L24" s="5"/>
     </row>
     <row r="25" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="20"/>
-      <c r="C25" s="14"/>
-      <c r="D25" s="9"/>
-      <c r="E25" s="10"/>
-      <c r="F25" s="10"/>
-      <c r="G25" s="10"/>
-      <c r="H25" s="7"/>
-      <c r="I25" s="7"/>
-      <c r="J25" s="7"/>
-      <c r="K25" s="7"/>
-      <c r="L25" s="8"/>
+      <c r="B25" s="15"/>
+      <c r="C25" s="11"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7"/>
+      <c r="G25" s="7"/>
+      <c r="H25" s="4"/>
+      <c r="I25" s="4"/>
+      <c r="J25" s="4"/>
+      <c r="K25" s="4"/>
+      <c r="L25" s="5"/>
     </row>
     <row r="26" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="20"/>
-      <c r="C26" s="14"/>
-      <c r="D26" s="9"/>
-      <c r="E26" s="10"/>
-      <c r="F26" s="10"/>
-      <c r="G26" s="10"/>
-      <c r="H26" s="11"/>
-      <c r="I26" s="7"/>
-      <c r="J26" s="7"/>
-      <c r="K26" s="7"/>
-      <c r="L26" s="8"/>
+      <c r="B26" s="15"/>
+      <c r="C26" s="11"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="7"/>
+      <c r="G26" s="7"/>
+      <c r="H26" s="4"/>
+      <c r="I26" s="4"/>
+      <c r="J26" s="4"/>
+      <c r="K26" s="4"/>
+      <c r="L26" s="5"/>
     </row>
     <row r="27" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="20"/>
-      <c r="C27" s="14"/>
-      <c r="D27" s="9"/>
-      <c r="E27" s="10"/>
-      <c r="F27" s="10"/>
-      <c r="G27" s="10"/>
-      <c r="H27" s="7"/>
-      <c r="I27" s="7"/>
-      <c r="J27" s="7"/>
-      <c r="K27" s="7"/>
-      <c r="L27" s="8"/>
+      <c r="B27" s="15"/>
+      <c r="C27" s="11"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="7"/>
+      <c r="F27" s="7"/>
+      <c r="G27" s="7"/>
+      <c r="H27" s="8"/>
+      <c r="I27" s="4"/>
+      <c r="J27" s="4"/>
+      <c r="K27" s="4"/>
+      <c r="L27" s="5"/>
     </row>
     <row r="28" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="20"/>
-      <c r="C28" s="14"/>
-      <c r="D28" s="9"/>
-      <c r="E28" s="10"/>
-      <c r="F28" s="10"/>
-      <c r="G28" s="10"/>
-      <c r="H28" s="7"/>
-      <c r="I28" s="7"/>
-      <c r="J28" s="7"/>
-      <c r="K28" s="7"/>
-      <c r="L28" s="8"/>
+      <c r="B28" s="15"/>
+      <c r="C28" s="11"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="7"/>
+      <c r="G28" s="7"/>
+      <c r="H28" s="4"/>
+      <c r="I28" s="4"/>
+      <c r="J28" s="4"/>
+      <c r="K28" s="4"/>
+      <c r="L28" s="5"/>
     </row>
     <row r="29" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="20"/>
-      <c r="C29" s="14"/>
-      <c r="D29" s="9"/>
-      <c r="E29" s="10"/>
-      <c r="F29" s="10"/>
-      <c r="G29" s="10"/>
-      <c r="H29" s="11"/>
-      <c r="I29" s="7"/>
-      <c r="J29" s="7"/>
-      <c r="K29" s="7"/>
-      <c r="L29" s="8"/>
+      <c r="B29" s="15"/>
+      <c r="C29" s="11"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="7"/>
+      <c r="F29" s="7"/>
+      <c r="G29" s="7"/>
+      <c r="H29" s="4"/>
+      <c r="I29" s="4"/>
+      <c r="J29" s="4"/>
+      <c r="K29" s="4"/>
+      <c r="L29" s="5"/>
     </row>
     <row r="30" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="20"/>
-      <c r="C30" s="14"/>
-      <c r="D30" s="9"/>
-      <c r="E30" s="10"/>
-      <c r="F30" s="10"/>
-      <c r="G30" s="10"/>
-      <c r="H30" s="7"/>
-      <c r="I30" s="7"/>
-      <c r="J30" s="7"/>
-      <c r="K30" s="7"/>
-      <c r="L30" s="8"/>
+      <c r="B30" s="15"/>
+      <c r="C30" s="11"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="7"/>
+      <c r="F30" s="7"/>
+      <c r="G30" s="7"/>
+      <c r="H30" s="4"/>
+      <c r="I30" s="4"/>
+      <c r="J30" s="4"/>
+      <c r="K30" s="4"/>
+      <c r="L30" s="5"/>
     </row>
     <row r="31" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C31" s="15"/>
+      <c r="B31" s="15"/>
+      <c r="C31" s="11"/>
+      <c r="D31" s="6"/>
+      <c r="E31" s="7"/>
+      <c r="F31" s="7"/>
+      <c r="G31" s="7"/>
+      <c r="H31" s="8"/>
+      <c r="I31" s="4"/>
+      <c r="J31" s="4"/>
+      <c r="K31" s="4"/>
+      <c r="L31" s="5"/>
     </row>
     <row r="32" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C32" s="15"/>
-    </row>
-    <row r="33" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C33" s="15"/>
-    </row>
-    <row r="34" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C34" s="15"/>
-    </row>
-    <row r="35" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C35" s="15"/>
-    </row>
-    <row r="36" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C36" s="15"/>
-    </row>
-    <row r="37" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C37" s="15"/>
-    </row>
-    <row r="38" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C38" s="15"/>
-    </row>
-    <row r="39" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C39" s="15"/>
-    </row>
-    <row r="40" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C40" s="15"/>
-    </row>
-    <row r="41" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C41" s="15"/>
-    </row>
-    <row r="42" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C42" s="15"/>
+      <c r="B32" s="15"/>
+      <c r="C32" s="11"/>
+      <c r="D32" s="6"/>
+      <c r="E32" s="7"/>
+      <c r="F32" s="7"/>
+      <c r="G32" s="7"/>
+      <c r="H32" s="4"/>
+      <c r="I32" s="4"/>
+      <c r="J32" s="4"/>
+      <c r="K32" s="4"/>
+      <c r="L32" s="5"/>
+    </row>
+    <row r="33" spans="2:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="15"/>
+      <c r="C33" s="11"/>
+      <c r="D33" s="6"/>
+      <c r="E33" s="7"/>
+      <c r="F33" s="7"/>
+      <c r="G33" s="7"/>
+      <c r="H33" s="4"/>
+      <c r="I33" s="4"/>
+      <c r="J33" s="4"/>
+      <c r="K33" s="4"/>
+      <c r="L33" s="5"/>
+    </row>
+    <row r="34" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B34" s="15"/>
+      <c r="C34" s="11"/>
+      <c r="D34" s="6"/>
+      <c r="E34" s="7"/>
+      <c r="F34" s="7"/>
+      <c r="G34" s="7"/>
+      <c r="H34" s="8"/>
+      <c r="I34" s="4"/>
+      <c r="J34" s="4"/>
+      <c r="K34" s="4"/>
+      <c r="L34" s="5"/>
+    </row>
+    <row r="35" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B35" s="15"/>
+      <c r="C35" s="11"/>
+      <c r="D35" s="6"/>
+      <c r="E35" s="7"/>
+      <c r="F35" s="7"/>
+      <c r="G35" s="7"/>
+      <c r="H35" s="4"/>
+      <c r="I35" s="4"/>
+      <c r="J35" s="4"/>
+      <c r="K35" s="4"/>
+      <c r="L35" s="5"/>
+    </row>
+    <row r="36" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B36" s="15"/>
+      <c r="C36" s="11"/>
+      <c r="D36" s="6"/>
+      <c r="E36" s="7"/>
+      <c r="F36" s="7"/>
+      <c r="G36" s="7"/>
+      <c r="H36" s="4"/>
+      <c r="I36" s="4"/>
+      <c r="J36" s="4"/>
+      <c r="K36" s="4"/>
+      <c r="L36" s="5"/>
+    </row>
+    <row r="37" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B37" s="15"/>
+      <c r="C37" s="11"/>
+      <c r="D37" s="6"/>
+      <c r="E37" s="7"/>
+      <c r="F37" s="7"/>
+      <c r="G37" s="7"/>
+      <c r="H37" s="4"/>
+      <c r="I37" s="4"/>
+      <c r="J37" s="4"/>
+      <c r="K37" s="4"/>
+      <c r="L37" s="5"/>
+    </row>
+    <row r="38" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B38" s="15"/>
+      <c r="C38" s="11"/>
+      <c r="D38" s="6"/>
+      <c r="E38" s="7"/>
+      <c r="F38" s="7"/>
+      <c r="G38" s="7"/>
+      <c r="H38" s="8"/>
+      <c r="I38" s="4"/>
+      <c r="J38" s="4"/>
+      <c r="K38" s="4"/>
+      <c r="L38" s="5"/>
+    </row>
+    <row r="39" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B39" s="15"/>
+      <c r="C39" s="11"/>
+      <c r="D39" s="6"/>
+      <c r="E39" s="7"/>
+      <c r="F39" s="7"/>
+      <c r="G39" s="7"/>
+      <c r="H39" s="4"/>
+      <c r="I39" s="4"/>
+      <c r="J39" s="4"/>
+      <c r="K39" s="4"/>
+      <c r="L39" s="5"/>
+    </row>
+    <row r="40" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B40" s="15"/>
+      <c r="C40" s="11"/>
+      <c r="D40" s="6"/>
+      <c r="E40" s="7"/>
+      <c r="F40" s="7"/>
+      <c r="G40" s="7"/>
+      <c r="H40" s="4"/>
+      <c r="I40" s="4"/>
+      <c r="J40" s="4"/>
+      <c r="K40" s="4"/>
+      <c r="L40" s="5"/>
+    </row>
+    <row r="41" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B41" s="15"/>
+      <c r="C41" s="11"/>
+      <c r="D41" s="6"/>
+      <c r="E41" s="7"/>
+      <c r="F41" s="7"/>
+      <c r="G41" s="7"/>
+      <c r="H41" s="8"/>
+      <c r="I41" s="4"/>
+      <c r="J41" s="4"/>
+      <c r="K41" s="4"/>
+      <c r="L41" s="5"/>
+    </row>
+    <row r="42" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B42" s="15"/>
+      <c r="C42" s="11"/>
+      <c r="D42" s="6"/>
+      <c r="E42" s="7"/>
+      <c r="F42" s="7"/>
+      <c r="G42" s="7"/>
+      <c r="H42" s="4"/>
+      <c r="I42" s="4"/>
+      <c r="J42" s="4"/>
+      <c r="K42" s="4"/>
+      <c r="L42" s="5"/>
+    </row>
+    <row r="43" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B43" s="15"/>
+      <c r="C43" s="11"/>
+      <c r="D43" s="6"/>
+      <c r="E43" s="7"/>
+      <c r="F43" s="7"/>
+      <c r="G43" s="7"/>
+      <c r="H43" s="4"/>
+      <c r="I43" s="4"/>
+      <c r="J43" s="4"/>
+      <c r="K43" s="4"/>
+      <c r="L43" s="5"/>
+    </row>
+    <row r="44" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B44" s="15"/>
+      <c r="C44" s="11"/>
+      <c r="D44" s="6"/>
+      <c r="E44" s="7"/>
+      <c r="F44" s="7"/>
+      <c r="G44" s="7"/>
+      <c r="H44" s="4"/>
+      <c r="I44" s="4"/>
+      <c r="J44" s="4"/>
+      <c r="K44" s="4"/>
+      <c r="L44" s="5"/>
+    </row>
+    <row r="45" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B45" s="15"/>
+      <c r="C45" s="11"/>
+      <c r="D45" s="6"/>
+      <c r="E45" s="7"/>
+      <c r="F45" s="7"/>
+      <c r="G45" s="7"/>
+      <c r="H45" s="4"/>
+      <c r="I45" s="4"/>
+      <c r="J45" s="4"/>
+      <c r="K45" s="4"/>
+      <c r="L45" s="5"/>
+    </row>
+    <row r="46" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B46" s="15"/>
+      <c r="C46" s="11"/>
+      <c r="D46" s="6"/>
+      <c r="E46" s="7"/>
+      <c r="F46" s="7"/>
+      <c r="G46" s="7"/>
+      <c r="H46" s="4"/>
+      <c r="I46" s="4"/>
+      <c r="J46" s="4"/>
+      <c r="K46" s="4"/>
+      <c r="L46" s="5"/>
+    </row>
+    <row r="47" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B47" s="15"/>
+      <c r="C47" s="11"/>
+      <c r="D47" s="6"/>
+      <c r="E47" s="7"/>
+      <c r="F47" s="7"/>
+      <c r="G47" s="7"/>
+      <c r="H47" s="8"/>
+      <c r="I47" s="4"/>
+      <c r="J47" s="4"/>
+      <c r="K47" s="4"/>
+      <c r="L47" s="5"/>
+    </row>
+    <row r="48" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B48" s="15"/>
+      <c r="C48" s="11"/>
+      <c r="D48" s="6"/>
+      <c r="E48" s="7"/>
+      <c r="F48" s="7"/>
+      <c r="G48" s="7"/>
+      <c r="H48" s="4"/>
+      <c r="I48" s="4"/>
+      <c r="J48" s="4"/>
+      <c r="K48" s="4"/>
+      <c r="L48" s="5"/>
+    </row>
+    <row r="49" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B49" s="15"/>
+      <c r="C49" s="11"/>
+      <c r="D49" s="6"/>
+      <c r="E49" s="7"/>
+      <c r="F49" s="7"/>
+      <c r="G49" s="7"/>
+      <c r="H49" s="4"/>
+      <c r="I49" s="4"/>
+      <c r="J49" s="4"/>
+      <c r="K49" s="4"/>
+      <c r="L49" s="5"/>
+    </row>
+    <row r="50" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B50" s="15"/>
+      <c r="C50" s="11"/>
+      <c r="D50" s="6"/>
+      <c r="E50" s="7"/>
+      <c r="F50" s="7"/>
+      <c r="G50" s="7"/>
+      <c r="H50" s="8"/>
+      <c r="I50" s="4"/>
+      <c r="J50" s="4"/>
+      <c r="K50" s="4"/>
+      <c r="L50" s="5"/>
+    </row>
+    <row r="51" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B51" s="15"/>
+      <c r="C51" s="11"/>
+      <c r="D51" s="6"/>
+      <c r="E51" s="7"/>
+      <c r="F51" s="7"/>
+      <c r="G51" s="7"/>
+      <c r="H51" s="4"/>
+      <c r="I51" s="4"/>
+      <c r="J51" s="4"/>
+      <c r="K51" s="4"/>
+      <c r="L51" s="5"/>
+    </row>
+    <row r="52" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B52" s="15"/>
+      <c r="C52" s="11"/>
+      <c r="D52" s="6"/>
+      <c r="E52" s="7"/>
+      <c r="F52" s="7"/>
+      <c r="G52" s="7"/>
+      <c r="H52" s="4"/>
+      <c r="I52" s="4"/>
+      <c r="J52" s="4"/>
+      <c r="K52" s="4"/>
+      <c r="L52" s="5"/>
+    </row>
+    <row r="53" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B53" s="15"/>
+      <c r="C53" s="11"/>
+      <c r="D53" s="6"/>
+      <c r="E53" s="7"/>
+      <c r="F53" s="7"/>
+      <c r="G53" s="7"/>
+      <c r="H53" s="4"/>
+      <c r="I53" s="4"/>
+      <c r="J53" s="4"/>
+      <c r="K53" s="4"/>
+      <c r="L53" s="5"/>
+    </row>
+    <row r="54" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B54" s="15"/>
+      <c r="C54" s="11"/>
+      <c r="D54" s="6"/>
+      <c r="E54" s="7"/>
+      <c r="F54" s="7"/>
+      <c r="G54" s="7"/>
+      <c r="H54" s="8"/>
+      <c r="I54" s="4"/>
+      <c r="J54" s="4"/>
+      <c r="K54" s="4"/>
+      <c r="L54" s="5"/>
+    </row>
+    <row r="55" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B55" s="15"/>
+      <c r="C55" s="11"/>
+      <c r="D55" s="6"/>
+      <c r="E55" s="7"/>
+      <c r="F55" s="7"/>
+      <c r="G55" s="7"/>
+      <c r="H55" s="4"/>
+      <c r="I55" s="4"/>
+      <c r="J55" s="4"/>
+      <c r="K55" s="4"/>
+      <c r="L55" s="5"/>
+    </row>
+    <row r="56" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B56" s="15"/>
+      <c r="C56" s="11"/>
+      <c r="D56" s="6"/>
+      <c r="E56" s="7"/>
+      <c r="F56" s="7"/>
+      <c r="G56" s="7"/>
+      <c r="H56" s="4"/>
+      <c r="I56" s="4"/>
+      <c r="J56" s="4"/>
+      <c r="K56" s="4"/>
+      <c r="L56" s="5"/>
+    </row>
+    <row r="57" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B57" s="15"/>
+      <c r="C57" s="11"/>
+      <c r="D57" s="6"/>
+      <c r="E57" s="7"/>
+      <c r="F57" s="7"/>
+      <c r="G57" s="7"/>
+      <c r="H57" s="8"/>
+      <c r="I57" s="4"/>
+      <c r="J57" s="4"/>
+      <c r="K57" s="4"/>
+      <c r="L57" s="5"/>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="D6:L6"/>
+    <mergeCell ref="B6:C6"/>
+  </mergeCells>
+  <conditionalFormatting sqref="F8:F17">
+    <cfRule type="top10" dxfId="7" priority="8" percent="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="6" priority="7" operator="greaterThan">
+      <formula>"average(f8:f17)"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="5" priority="6" operator="greaterThan">
+      <formula>"average(f8:f17)"</formula>
+    </cfRule>
+    <cfRule type="top10" dxfId="4" priority="5" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="3" priority="4" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="2" priority="3" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E8:E17">
+    <cfRule type="top10" dxfId="1" priority="2" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G8:G17">
+    <cfRule type="top10" dxfId="0" priority="1" percent="1" rank="10"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>

</xml_diff>